<commit_message>
Update Ssks excel examplar (#1081)
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssks_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssks_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\PlanPro\PlanPro-Wzk-60.18.0\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A71D75-8006-4B0A-BE69-72DE009EBB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C114D90-3923-4088-9E8A-46DDAB013705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,10 +332,6 @@
 Sh 1</t>
   </si>
   <si>
-    <t>Abstand
-Mastmitte - Gleismitte</t>
-  </si>
-  <si>
     <t>Bezeichnung Signal</t>
   </si>
   <si>
@@ -385,6 +381,11 @@
   <si>
     <t>Dunkel-
 schaltung</t>
+  </si>
+  <si>
+    <t>Abstand
+Mastmitte - Gleismitte
+(Gleisabstand)</t>
   </si>
 </sst>
 </file>
@@ -851,6 +852,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -876,9 +880,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1257,7 +1258,7 @@
   <dimension ref="A1:AY557"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1449,77 +1450,77 @@
         <v>47</v>
       </c>
       <c r="AX1" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AY1" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:51" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
       <c r="B2" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="47" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="47" t="s">
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="47" t="s">
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="47" t="s">
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
-      <c r="AR2" s="47" t="s">
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="49"/>
+      <c r="AP2" s="49"/>
+      <c r="AQ2" s="49"/>
+      <c r="AR2" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="AS2" s="48"/>
-      <c r="AT2" s="48"/>
-      <c r="AU2" s="48"/>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="49"/>
+      <c r="AS2" s="49"/>
+      <c r="AT2" s="49"/>
+      <c r="AU2" s="49"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="50"/>
       <c r="AY2" s="20" t="s">
         <v>53</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>55</v>
@@ -1539,98 +1540,98 @@
       <c r="F3" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="44"/>
+      <c r="G3" s="45"/>
       <c r="H3" s="6" t="s">
         <v>57</v>
       </c>
       <c r="I3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="L3" s="44"/>
-      <c r="M3" s="45" t="s">
+      <c r="K3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="53"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="45" t="s">
+      <c r="N3" s="44"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="46"/>
+      <c r="Q3" s="47"/>
       <c r="R3" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="S3" s="44"/>
+      <c r="S3" s="45"/>
       <c r="T3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="U3" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="U3" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="44"/>
-      <c r="W3" s="45" t="s">
+      <c r="V3" s="45"/>
+      <c r="W3" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="X3" s="46"/>
+      <c r="X3" s="47"/>
       <c r="Y3" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="Z3" s="44"/>
+      <c r="Z3" s="45"/>
       <c r="AA3" s="6" t="s">
         <v>93</v>
       </c>
       <c r="AB3" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC3" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="45" t="s">
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="45"/>
+      <c r="AH3" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="53"/>
-      <c r="AN3" s="44"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="44"/>
+      <c r="AL3" s="44"/>
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="45"/>
       <c r="AO3" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AP3" s="6" t="s">
         <v>66</v>
       </c>
       <c r="AQ3" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR3" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS3" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="AR3" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="AS3" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="AT3" s="6" t="s">
         <v>67</v>
       </c>
       <c r="AU3" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AV3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="AW3" s="45" t="s">
+      <c r="AW3" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="AX3" s="46"/>
+      <c r="AX3" s="47"/>
       <c r="AY3" s="31"/>
     </row>
     <row r="4" spans="1:51" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1683,7 +1684,7 @@
         <v>79</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X4" s="12" t="s">
         <v>80</v>
@@ -2535,23 +2536,23 @@
     <row r="557" s="22" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="AH3:AN3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:Q2"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="AC2:AQ2"/>
     <mergeCell ref="AC3:AG3"/>
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="W3:X3"/>
     <mergeCell ref="AR2:AX2"/>
     <mergeCell ref="U3:V3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:Q2"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="AC2:AQ2"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="AH3:AN3"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -2563,52 +2564,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -2800,28 +2768,69 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5608CC1-62E8-40C3-93D3-D4A0440D7ADA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E76690F-8A23-45F3-AC2B-ADA60E406AB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F25B32D-FD26-4105-AE41-4DDE11D43643}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CD9C34-55B9-46DF-94B7-6C19782F39DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2840,18 +2849,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F25B32D-FD26-4105-AE41-4DDE11D43643}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5608CC1-62E8-40C3-93D3-D4A0440D7ADA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E76690F-8A23-45F3-AC2B-ADA60E406AB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>